<commit_message>
docs: :memo: Update ReadMe and xlsx
</commit_message>
<xml_diff>
--- a/ASI2 Framework Frontend Cours.xlsx
+++ b/ASI2 Framework Frontend Cours.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11210"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1D16004-D11E-E341-9CAE-ACDA11C23D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F006EA-F222-0A42-A46C-2248469F874C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -380,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -410,25 +410,34 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -440,12 +449,30 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -466,20 +493,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
@@ -494,21 +507,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FFFF5050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -522,14 +528,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -841,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="109" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -856,26 +855,26 @@
       </c>
       <c r="E1" s="17"/>
       <c r="F1" s="6"/>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="15" t="s">
         <v>58</v>
       </c>
       <c r="H1" s="17"/>
       <c r="I1" s="6"/>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="15" t="s">
         <v>57</v>
       </c>
       <c r="K1" s="17"/>
       <c r="L1" s="7"/>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="15" t="s">
         <v>56</v>
       </c>
       <c r="N1" s="17"/>
       <c r="O1" s="7"/>
-      <c r="P1" s="18" t="s">
+      <c r="P1" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="D2" s="2" t="s">
@@ -947,40 +946,40 @@
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="5">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="E4" s="5">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="F4" s="5">
-        <v>0</v>
-      </c>
-      <c r="G4" s="12">
-        <v>0.1</v>
+        <v>0.25</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.25</v>
       </c>
       <c r="H4" s="5">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="I4" s="5">
-        <v>0</v>
-      </c>
-      <c r="J4" s="12">
-        <v>0.4</v>
+        <v>0.25</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0.25</v>
       </c>
       <c r="K4" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="L4" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="M4" s="12">
-        <v>0.4</v>
+        <v>0.25</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0.25</v>
       </c>
       <c r="N4" s="5">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="O4" s="13">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="P4" s="12">
         <f>D4+G4+J4+M4</f>
@@ -988,7 +987,7 @@
       </c>
       <c r="Q4" s="5">
         <f>E4+H4+K4+N4</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="R4" s="5">
         <f>F4+I4+L4+O4</f>
@@ -996,11 +995,11 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -1019,10 +1018,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="16"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -1049,37 +1048,37 @@
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" t="s">
-        <v>14</v>
+      <c r="H7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" s="15" t="s">
-        <v>14</v>
+      <c r="K7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O7" s="15" t="s">
-        <v>14</v>
+      <c r="N7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -1092,37 +1091,37 @@
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" t="s">
-        <v>14</v>
+      <c r="H8" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" s="15" t="s">
-        <v>14</v>
+      <c r="K8" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N8" t="s">
-        <v>14</v>
-      </c>
-      <c r="O8" s="15" t="s">
-        <v>14</v>
+      <c r="N8" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
@@ -1135,37 +1134,37 @@
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" t="s">
-        <v>14</v>
+      <c r="H9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K9" t="s">
-        <v>14</v>
-      </c>
-      <c r="L9" s="15" t="s">
-        <v>14</v>
+      <c r="K9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N9" t="s">
-        <v>14</v>
-      </c>
-      <c r="O9" s="15" t="s">
-        <v>14</v>
+      <c r="N9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -1178,37 +1177,37 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G10" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" t="s">
-        <v>14</v>
+      <c r="H10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10" s="15" t="s">
-        <v>14</v>
+      <c r="K10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M10" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N10" t="s">
-        <v>14</v>
-      </c>
-      <c r="O10" s="15" t="s">
-        <v>14</v>
+      <c r="N10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="27" x14ac:dyDescent="0.2">
@@ -1221,37 +1220,37 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H11" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" t="s">
-        <v>14</v>
+      <c r="H11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="15" t="s">
-        <v>14</v>
+      <c r="K11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N11" t="s">
-        <v>14</v>
-      </c>
-      <c r="O11" s="15" t="s">
-        <v>14</v>
+      <c r="N11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="27" x14ac:dyDescent="0.2">
@@ -1264,37 +1263,37 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" t="s">
-        <v>14</v>
+      <c r="H12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K12" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" s="15" t="s">
-        <v>14</v>
+      <c r="K12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N12" t="s">
-        <v>14</v>
-      </c>
-      <c r="O12" s="15" t="s">
-        <v>14</v>
+      <c r="N12" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="O12" s="14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -1307,37 +1306,37 @@
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" t="s">
-        <v>14</v>
+      <c r="H13" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="J13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K13" t="s">
-        <v>14</v>
-      </c>
-      <c r="L13" s="15" t="s">
-        <v>14</v>
+      <c r="K13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N13" t="s">
-        <v>14</v>
-      </c>
-      <c r="O13" s="15" t="s">
-        <v>14</v>
+      <c r="N13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O13" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="27" x14ac:dyDescent="0.2">
@@ -1350,37 +1349,37 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G14" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" t="s">
-        <v>14</v>
+      <c r="H14" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J14" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K14" t="s">
-        <v>14</v>
-      </c>
-      <c r="L14" s="15" t="s">
-        <v>14</v>
+      <c r="K14" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M14" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N14" t="s">
-        <v>14</v>
-      </c>
-      <c r="O14" s="15" t="s">
-        <v>14</v>
+      <c r="N14" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O14" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
@@ -1393,37 +1392,37 @@
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G15" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H15" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" t="s">
-        <v>14</v>
+      <c r="H15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J15" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K15" t="s">
-        <v>14</v>
-      </c>
-      <c r="L15" s="15" t="s">
-        <v>14</v>
+      <c r="K15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M15" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N15" t="s">
-        <v>14</v>
-      </c>
-      <c r="O15" s="15" t="s">
-        <v>14</v>
+      <c r="N15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O15" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="27" x14ac:dyDescent="0.2">
@@ -1436,37 +1435,37 @@
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G16" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H16" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" t="s">
-        <v>14</v>
+      <c r="H16" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J16" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K16" t="s">
-        <v>14</v>
-      </c>
-      <c r="L16" s="15" t="s">
-        <v>14</v>
+      <c r="K16" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M16" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N16" t="s">
-        <v>14</v>
-      </c>
-      <c r="O16" s="15" t="s">
-        <v>14</v>
+      <c r="N16" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O16" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
@@ -1479,37 +1478,37 @@
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G17" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I17" t="s">
-        <v>14</v>
+      <c r="H17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J17" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K17" t="s">
-        <v>14</v>
-      </c>
-      <c r="L17" s="15" t="s">
-        <v>14</v>
+      <c r="K17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M17" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N17" t="s">
-        <v>14</v>
-      </c>
-      <c r="O17" s="15" t="s">
-        <v>14</v>
+      <c r="N17" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O17" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -1522,37 +1521,37 @@
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F18" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" t="s">
-        <v>14</v>
+      <c r="H18" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K18" t="s">
-        <v>14</v>
-      </c>
-      <c r="L18" s="15" t="s">
-        <v>14</v>
+      <c r="K18" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L18" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N18" t="s">
-        <v>14</v>
-      </c>
-      <c r="O18" s="15" t="s">
-        <v>14</v>
+      <c r="N18" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O18" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="27" x14ac:dyDescent="0.2">
@@ -1565,37 +1564,37 @@
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G19" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H19" t="s">
-        <v>14</v>
-      </c>
-      <c r="I19" t="s">
-        <v>14</v>
+      <c r="H19" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J19" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K19" t="s">
-        <v>14</v>
-      </c>
-      <c r="L19" s="15" t="s">
-        <v>14</v>
+      <c r="K19" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L19" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M19" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N19" t="s">
-        <v>14</v>
-      </c>
-      <c r="O19" s="15" t="s">
-        <v>14</v>
+      <c r="N19" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O19" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
@@ -1608,37 +1607,37 @@
         <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G20" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H20" t="s">
-        <v>14</v>
-      </c>
-      <c r="I20" t="s">
-        <v>14</v>
+      <c r="H20" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J20" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K20" t="s">
-        <v>14</v>
-      </c>
-      <c r="L20" s="15" t="s">
-        <v>14</v>
+      <c r="K20" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L20" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M20" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N20" t="s">
-        <v>14</v>
-      </c>
-      <c r="O20" s="15" t="s">
-        <v>14</v>
+      <c r="N20" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O20" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -1651,37 +1650,37 @@
         <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G21" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H21" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" t="s">
-        <v>14</v>
+      <c r="H21" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J21" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K21" t="s">
-        <v>14</v>
-      </c>
-      <c r="L21" s="15" t="s">
-        <v>14</v>
+      <c r="K21" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L21" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="M21" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N21" t="s">
-        <v>14</v>
-      </c>
-      <c r="O21" s="15" t="s">
-        <v>14</v>
+      <c r="N21" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O21" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
@@ -1694,37 +1693,37 @@
         <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G22" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H22" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" t="s">
-        <v>14</v>
+      <c r="H22" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J22" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K22" t="s">
-        <v>14</v>
-      </c>
-      <c r="L22" s="15" t="s">
-        <v>14</v>
+      <c r="K22" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L22" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M22" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N22" t="s">
-        <v>14</v>
-      </c>
-      <c r="O22" s="15" t="s">
-        <v>14</v>
+      <c r="N22" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O22" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="27" x14ac:dyDescent="0.2">
@@ -1737,37 +1736,37 @@
         <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G23" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H23" t="s">
-        <v>14</v>
-      </c>
-      <c r="I23" t="s">
-        <v>14</v>
+      <c r="H23" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J23" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K23" t="s">
-        <v>14</v>
-      </c>
-      <c r="L23" s="15" t="s">
-        <v>14</v>
+      <c r="K23" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L23" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M23" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N23" t="s">
-        <v>14</v>
-      </c>
-      <c r="O23" s="15" t="s">
-        <v>14</v>
+      <c r="N23" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O23" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="27" x14ac:dyDescent="0.2">
@@ -1780,37 +1779,37 @@
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G24" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H24" t="s">
-        <v>14</v>
-      </c>
-      <c r="I24" t="s">
-        <v>14</v>
+      <c r="H24" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J24" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K24" t="s">
-        <v>14</v>
-      </c>
-      <c r="L24" s="15" t="s">
-        <v>14</v>
+      <c r="K24" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L24" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M24" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N24" t="s">
-        <v>14</v>
-      </c>
-      <c r="O24" s="15" t="s">
-        <v>14</v>
+      <c r="N24" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O24" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -1823,45 +1822,45 @@
         <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G25" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H25" t="s">
-        <v>14</v>
-      </c>
-      <c r="I25" t="s">
-        <v>14</v>
+      <c r="H25" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I25" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="J25" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K25" t="s">
-        <v>14</v>
-      </c>
-      <c r="L25" s="15" t="s">
-        <v>14</v>
+      <c r="K25" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L25" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M25" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N25" t="s">
-        <v>14</v>
-      </c>
-      <c r="O25" s="15" t="s">
-        <v>14</v>
+      <c r="N25" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O25" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="16"/>
+      <c r="C26" s="19"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -1885,37 +1884,37 @@
         <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G27" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H27" t="s">
-        <v>14</v>
-      </c>
-      <c r="I27" t="s">
-        <v>14</v>
+      <c r="H27" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J27" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K27" t="s">
-        <v>14</v>
-      </c>
-      <c r="L27" s="15" t="s">
-        <v>14</v>
+      <c r="K27" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L27" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M27" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N27" t="s">
-        <v>14</v>
-      </c>
-      <c r="O27" s="15" t="s">
-        <v>14</v>
+      <c r="N27" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O27" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
@@ -1928,37 +1927,37 @@
         <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F28" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G28" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H28" t="s">
-        <v>14</v>
-      </c>
-      <c r="I28" t="s">
-        <v>14</v>
+      <c r="H28" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J28" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K28" t="s">
-        <v>14</v>
-      </c>
-      <c r="L28" s="15" t="s">
-        <v>14</v>
+      <c r="K28" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L28" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M28" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N28" t="s">
-        <v>14</v>
-      </c>
-      <c r="O28" s="15" t="s">
-        <v>14</v>
+      <c r="N28" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O28" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
@@ -1971,37 +1970,37 @@
         <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F29" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G29" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H29" t="s">
-        <v>14</v>
-      </c>
-      <c r="I29" t="s">
-        <v>14</v>
+      <c r="H29" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J29" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K29" t="s">
-        <v>14</v>
-      </c>
-      <c r="L29" s="15" t="s">
-        <v>14</v>
+      <c r="K29" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L29" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M29" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N29" t="s">
-        <v>14</v>
-      </c>
-      <c r="O29" s="15" t="s">
-        <v>14</v>
+      <c r="N29" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O29" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
@@ -2014,37 +2013,37 @@
         <v>10</v>
       </c>
       <c r="E30" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F30" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G30" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H30" t="s">
-        <v>14</v>
-      </c>
-      <c r="I30" t="s">
-        <v>14</v>
+      <c r="H30" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J30" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K30" t="s">
-        <v>14</v>
-      </c>
-      <c r="L30" s="15" t="s">
-        <v>14</v>
+      <c r="K30" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L30" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M30" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N30" t="s">
-        <v>14</v>
-      </c>
-      <c r="O30" s="15" t="s">
-        <v>14</v>
+      <c r="N30" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O30" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="27" x14ac:dyDescent="0.2">
@@ -2057,37 +2056,37 @@
         <v>10</v>
       </c>
       <c r="E31" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F31" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G31" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H31" t="s">
-        <v>14</v>
-      </c>
-      <c r="I31" t="s">
-        <v>14</v>
+      <c r="H31" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I31" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J31" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K31" t="s">
-        <v>14</v>
-      </c>
-      <c r="L31" s="15" t="s">
-        <v>14</v>
+      <c r="K31" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L31" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M31" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N31" t="s">
-        <v>14</v>
-      </c>
-      <c r="O31" s="15" t="s">
-        <v>14</v>
+      <c r="N31" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O31" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
@@ -2100,37 +2099,37 @@
         <v>10</v>
       </c>
       <c r="E32" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G32" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H32" t="s">
-        <v>14</v>
-      </c>
-      <c r="I32" t="s">
-        <v>14</v>
+      <c r="H32" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I32" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J32" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K32" t="s">
-        <v>14</v>
-      </c>
-      <c r="L32" s="15" t="s">
-        <v>14</v>
+      <c r="K32" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L32" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M32" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="N32" t="s">
-        <v>14</v>
-      </c>
-      <c r="O32" s="15" t="s">
-        <v>14</v>
+      <c r="N32" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="O32" s="14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
@@ -2143,37 +2142,37 @@
         <v>10</v>
       </c>
       <c r="E33" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F33" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G33" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H33" t="s">
-        <v>14</v>
-      </c>
-      <c r="I33" t="s">
-        <v>14</v>
+      <c r="H33" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J33" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K33" t="s">
-        <v>14</v>
-      </c>
-      <c r="L33" s="15" t="s">
-        <v>14</v>
+      <c r="K33" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L33" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M33" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="N33" t="s">
-        <v>14</v>
-      </c>
-      <c r="O33" s="15" t="s">
-        <v>14</v>
+      <c r="N33" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="O33" s="14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2186,37 +2185,37 @@
         <v>10</v>
       </c>
       <c r="E34" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F34" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G34" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H34" t="s">
-        <v>14</v>
-      </c>
-      <c r="I34" t="s">
-        <v>14</v>
+      <c r="H34" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J34" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K34" t="s">
-        <v>14</v>
-      </c>
-      <c r="L34" s="15" t="s">
-        <v>14</v>
+      <c r="K34" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L34" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M34" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="N34" t="s">
-        <v>14</v>
-      </c>
-      <c r="O34" s="15" t="s">
-        <v>14</v>
+      <c r="N34" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="O34" s="14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
@@ -2229,37 +2228,37 @@
         <v>10</v>
       </c>
       <c r="E35" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F35" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G35" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H35" t="s">
-        <v>14</v>
-      </c>
-      <c r="I35" t="s">
-        <v>14</v>
+      <c r="H35" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I35" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J35" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K35" t="s">
-        <v>14</v>
-      </c>
-      <c r="L35" s="15" t="s">
-        <v>14</v>
+      <c r="K35" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L35" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M35" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="N35" t="s">
-        <v>14</v>
-      </c>
-      <c r="O35" s="15" t="s">
-        <v>14</v>
+      <c r="N35" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="O35" s="14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="27" x14ac:dyDescent="0.2">
@@ -2272,37 +2271,37 @@
         <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F36" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G36" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H36" t="s">
-        <v>14</v>
-      </c>
-      <c r="I36" t="s">
-        <v>14</v>
+      <c r="H36" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J36" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K36" t="s">
-        <v>14</v>
-      </c>
-      <c r="L36" s="15" t="s">
-        <v>14</v>
+      <c r="K36" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L36" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M36" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N36" t="s">
-        <v>14</v>
-      </c>
-      <c r="O36" s="15" t="s">
-        <v>14</v>
+      <c r="N36" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O36" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="27" x14ac:dyDescent="0.2">
@@ -2315,37 +2314,37 @@
         <v>10</v>
       </c>
       <c r="E37" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F37" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G37" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H37" t="s">
-        <v>14</v>
-      </c>
-      <c r="I37" t="s">
-        <v>14</v>
+      <c r="H37" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I37" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J37" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K37" t="s">
-        <v>14</v>
-      </c>
-      <c r="L37" s="15" t="s">
-        <v>14</v>
+      <c r="K37" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L37" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="M37" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N37" t="s">
-        <v>14</v>
-      </c>
-      <c r="O37" s="15" t="s">
-        <v>14</v>
+      <c r="N37" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O37" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
@@ -2358,37 +2357,37 @@
         <v>10</v>
       </c>
       <c r="E38" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F38" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G38" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H38" t="s">
-        <v>14</v>
-      </c>
-      <c r="I38" t="s">
-        <v>14</v>
+      <c r="H38" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J38" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K38" t="s">
-        <v>14</v>
-      </c>
-      <c r="L38" s="15" t="s">
-        <v>14</v>
+      <c r="K38" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L38" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M38" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N38" t="s">
-        <v>14</v>
-      </c>
-      <c r="O38" s="15" t="s">
-        <v>14</v>
+      <c r="N38" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O38" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="27" x14ac:dyDescent="0.2">
@@ -2401,37 +2400,37 @@
         <v>10</v>
       </c>
       <c r="E39" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F39" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G39" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H39" t="s">
-        <v>14</v>
-      </c>
-      <c r="I39" t="s">
-        <v>14</v>
+      <c r="H39" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I39" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="J39" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K39" t="s">
-        <v>14</v>
-      </c>
-      <c r="L39" s="15" t="s">
-        <v>14</v>
+      <c r="K39" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L39" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M39" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N39" t="s">
-        <v>14</v>
-      </c>
-      <c r="O39" s="15" t="s">
-        <v>14</v>
+      <c r="N39" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O39" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
@@ -2444,37 +2443,37 @@
         <v>10</v>
       </c>
       <c r="E40" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F40" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G40" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H40" t="s">
-        <v>14</v>
-      </c>
-      <c r="I40" t="s">
-        <v>14</v>
+      <c r="H40" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I40" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J40" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K40" t="s">
-        <v>14</v>
-      </c>
-      <c r="L40" s="15" t="s">
-        <v>14</v>
+      <c r="K40" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L40" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M40" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N40" t="s">
-        <v>14</v>
-      </c>
-      <c r="O40" s="15" t="s">
-        <v>14</v>
+      <c r="N40" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O40" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="27" x14ac:dyDescent="0.2">
@@ -2487,37 +2486,37 @@
         <v>10</v>
       </c>
       <c r="E41" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F41" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G41" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H41" t="s">
-        <v>14</v>
-      </c>
-      <c r="I41" t="s">
-        <v>14</v>
+      <c r="H41" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I41" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="J41" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K41" t="s">
-        <v>14</v>
-      </c>
-      <c r="L41" s="15" t="s">
-        <v>14</v>
+      <c r="K41" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L41" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="M41" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N41" t="s">
-        <v>14</v>
-      </c>
-      <c r="O41" s="15" t="s">
-        <v>14</v>
+      <c r="N41" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="O41" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2530,37 +2529,37 @@
         <v>10</v>
       </c>
       <c r="E42" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F42" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G42" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H42" t="s">
-        <v>14</v>
-      </c>
-      <c r="I42" t="s">
-        <v>14</v>
+      <c r="H42" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I42" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="J42" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K42" t="s">
-        <v>14</v>
-      </c>
-      <c r="L42" s="15" t="s">
-        <v>14</v>
+      <c r="K42" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L42" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="M42" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N42" t="s">
-        <v>14</v>
-      </c>
-      <c r="O42" s="15" t="s">
-        <v>14</v>
+      <c r="N42" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="O42" s="14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2573,37 +2572,37 @@
         <v>10</v>
       </c>
       <c r="E43" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F43" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G43" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H43" t="s">
-        <v>14</v>
-      </c>
-      <c r="I43" t="s">
-        <v>14</v>
+      <c r="H43" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I43" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="J43" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K43" t="s">
-        <v>14</v>
-      </c>
-      <c r="L43" s="15" t="s">
-        <v>14</v>
+      <c r="K43" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L43" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="M43" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N43" t="s">
-        <v>14</v>
-      </c>
-      <c r="O43" s="15" t="s">
-        <v>14</v>
+      <c r="N43" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="O43" s="14" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2641,50 +2640,50 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:O25">
-    <cfRule type="cellIs" dxfId="13" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="33" operator="equal">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="34" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="36" operator="equal">
       <formula>"-"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="35" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="34" operator="equal">
-      <formula>"C"</formula>
+    <cfRule type="cellIs" dxfId="9" priority="31" operator="equal">
+      <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="33" operator="equal">
-      <formula>"B"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="32" operator="equal">
       <formula>"AB"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="31" operator="equal">
-      <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:O43">
-    <cfRule type="cellIs" dxfId="7" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="21" operator="equal">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="22" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="24" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="23" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="19" operator="equal">
       <formula>"A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="20" operator="equal">
       <formula>"AB"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="23" operator="equal">
-      <formula>"D"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="24" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="21" operator="equal">
-      <formula>"B"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="22" operator="equal">
-      <formula>"C"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:R4">
-    <cfRule type="cellIs" dxfId="1" priority="109" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="110" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="109" operator="notEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>